<commit_message>
Corrected reference designators, added bar codes where necessary
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CE01ISSP_00004.xlsx
+++ b/deployment/Omaha_Cal_Info_CE01ISSP_00004.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\# OOI_Asset_Management\CE_mod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1872" yWindow="948" windowWidth="25608" windowHeight="16068" tabRatio="579"/>
+    <workbookView xWindow="1875" yWindow="945" windowWidth="25605" windowHeight="16065" tabRatio="579" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -1270,7 +1270,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1371,6 +1371,7 @@
     <xf numFmtId="0" fontId="34" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="15" fontId="25" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="528">
     <cellStyle name="Comma 2" xfId="3"/>
@@ -2256,28 +2257,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" customWidth="1"/>
-    <col min="13" max="13" width="15.109375" customWidth="1"/>
-    <col min="14" max="14" width="13.88671875" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="6" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>101</v>
       </c>
@@ -2315,7 +2316,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>112</v>
       </c>
@@ -2334,7 +2335,9 @@
       <c r="F2" s="41">
         <v>0.93055555555555547</v>
       </c>
-      <c r="G2" s="39"/>
+      <c r="G2" s="46">
+        <v>42536</v>
+      </c>
       <c r="H2" s="39" t="s">
         <v>90</v>
       </c>
@@ -2356,13 +2359,13 @@
         <v>-124.09524</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="11"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D4" s="9"/>
       <c r="E4" s="10"/>
       <c r="F4" s="11"/>
@@ -2371,7 +2374,7 @@
         <v>44.656019999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D5" s="9"/>
       <c r="E5" s="10"/>
       <c r="F5" s="11"/>
@@ -2380,73 +2383,73 @@
         <v>-124.09524</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D6" s="9"/>
       <c r="E6" s="10"/>
       <c r="F6" s="11"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D7" s="9"/>
       <c r="E7" s="10"/>
       <c r="F7" s="11"/>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D8" s="9"/>
       <c r="E8" s="10"/>
       <c r="F8" s="11"/>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D9" s="9"/>
       <c r="E9" s="10"/>
       <c r="F9" s="11"/>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D10" s="9"/>
       <c r="E10" s="10"/>
       <c r="F10" s="11"/>
       <c r="G10" s="10"/>
     </row>
-    <row r="11" spans="1:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D11" s="9"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="1:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D12" s="9"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D13" s="9"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="1:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D14" s="9"/>
       <c r="E14" s="10"/>
       <c r="F14" s="11"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="1:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D15" s="9"/>
       <c r="E15" s="10"/>
       <c r="F15" s="11"/>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="1:14" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D16" s="9"/>
       <c r="E16" s="10"/>
       <c r="F16" s="11"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="4:7" s="8" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:7" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="D17" s="9"/>
       <c r="E17" s="10"/>
       <c r="F17" s="11"/>
@@ -2468,25 +2471,25 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" customWidth="1"/>
-    <col min="4" max="5" width="12.44140625" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="5" width="12.42578125" customWidth="1"/>
     <col min="6" max="6" width="17" style="7" customWidth="1"/>
-    <col min="7" max="7" width="37.88671875" customWidth="1"/>
-    <col min="8" max="8" width="57.33203125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="21.33203125" customWidth="1"/>
+    <col min="7" max="7" width="37.85546875" customWidth="1"/>
+    <col min="8" max="8" width="57.28515625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2515,7 +2518,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -2526,7 +2529,7 @@
       <c r="H2" s="16"/>
       <c r="I2" s="17"/>
     </row>
-    <row r="3" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>91</v>
       </c>
@@ -2555,7 +2558,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>91</v>
       </c>
@@ -2584,7 +2587,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>91</v>
       </c>
@@ -2613,7 +2616,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>91</v>
       </c>
@@ -2642,7 +2645,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7" s="18"/>
       <c r="C7" s="23"/>
@@ -2653,7 +2656,7 @@
       <c r="H7" s="21"/>
       <c r="I7" s="16"/>
     </row>
-    <row r="8" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>92</v>
       </c>
@@ -2682,7 +2685,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>92</v>
       </c>
@@ -2709,7 +2712,7 @@
       </c>
       <c r="I9" s="27"/>
     </row>
-    <row r="10" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>92</v>
       </c>
@@ -2736,7 +2739,7 @@
       </c>
       <c r="I10" s="27"/>
     </row>
-    <row r="11" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>92</v>
       </c>
@@ -2763,7 +2766,7 @@
       </c>
       <c r="I11" s="27"/>
     </row>
-    <row r="12" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>92</v>
       </c>
@@ -2790,7 +2793,7 @@
       </c>
       <c r="I12" s="27"/>
     </row>
-    <row r="13" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>92</v>
       </c>
@@ -2817,7 +2820,7 @@
       </c>
       <c r="I13" s="27"/>
     </row>
-    <row r="14" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>92</v>
       </c>
@@ -2844,7 +2847,7 @@
       </c>
       <c r="I14" s="27"/>
     </row>
-    <row r="15" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>92</v>
       </c>
@@ -2871,7 +2874,7 @@
       </c>
       <c r="I15" s="27"/>
     </row>
-    <row r="16" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
       <c r="C16" s="23"/>
@@ -2882,7 +2885,7 @@
       <c r="H16" s="21"/>
       <c r="I16" s="16"/>
     </row>
-    <row r="17" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>93</v>
       </c>
@@ -2911,7 +2914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>93</v>
       </c>
@@ -2940,7 +2943,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19"/>
       <c r="C19" s="23"/>
@@ -2951,7 +2954,7 @@
       <c r="H19" s="21"/>
       <c r="I19" s="16"/>
     </row>
-    <row r="20" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>94</v>
       </c>
@@ -2980,7 +2983,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>94</v>
       </c>
@@ -3009,7 +3012,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>94</v>
       </c>
@@ -3038,7 +3041,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>94</v>
       </c>
@@ -3067,7 +3070,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>94</v>
       </c>
@@ -3096,7 +3099,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>94</v>
       </c>
@@ -3125,7 +3128,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>94</v>
       </c>
@@ -3154,7 +3157,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="23"/>
@@ -3165,7 +3168,7 @@
       <c r="H27" s="21"/>
       <c r="I27" s="16"/>
     </row>
-    <row r="28" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>95</v>
       </c>
@@ -3192,7 +3195,7 @@
       </c>
       <c r="I28" s="16"/>
     </row>
-    <row r="29" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
         <v>95</v>
       </c>
@@ -3219,7 +3222,7 @@
       </c>
       <c r="I29" s="16"/>
     </row>
-    <row r="30" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
         <v>95</v>
       </c>
@@ -3246,7 +3249,7 @@
       </c>
       <c r="I30" s="16"/>
     </row>
-    <row r="31" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
       <c r="B31" s="18"/>
       <c r="C31" s="23"/>
@@ -3257,7 +3260,7 @@
       <c r="H31" s="21"/>
       <c r="I31" s="16"/>
     </row>
-    <row r="32" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>96</v>
       </c>
@@ -3286,7 +3289,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
         <v>96</v>
       </c>
@@ -3315,7 +3318,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
         <v>96</v>
       </c>
@@ -3344,7 +3347,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
         <v>96</v>
       </c>
@@ -3373,7 +3376,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
         <v>96</v>
       </c>
@@ -3402,7 +3405,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>96</v>
       </c>
@@ -3431,7 +3434,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
         <v>96</v>
       </c>
@@ -3460,7 +3463,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
         <v>96</v>
       </c>
@@ -3489,7 +3492,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
         <v>96</v>
       </c>
@@ -3518,7 +3521,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
         <v>96</v>
       </c>
@@ -3547,7 +3550,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="22"/>
       <c r="B42" s="22"/>
       <c r="C42" s="23"/>
@@ -3558,7 +3561,7 @@
       <c r="H42" s="21"/>
       <c r="I42" s="16"/>
     </row>
-    <row r="43" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
         <v>97</v>
       </c>
@@ -3587,7 +3590,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
         <v>97</v>
       </c>
@@ -3616,7 +3619,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="18"/>
       <c r="B45" s="18"/>
       <c r="C45" s="23"/>
@@ -3627,7 +3630,7 @@
       <c r="H45" s="21"/>
       <c r="I45" s="16"/>
     </row>
-    <row r="46" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
         <v>98</v>
       </c>
@@ -3654,7 +3657,7 @@
       </c>
       <c r="I46" s="16"/>
     </row>
-    <row r="47" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
         <v>98</v>
       </c>
@@ -3681,7 +3684,7 @@
       </c>
       <c r="I47" s="16"/>
     </row>
-    <row r="48" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
         <v>98</v>
       </c>
@@ -3708,7 +3711,7 @@
       </c>
       <c r="I48" s="16"/>
     </row>
-    <row r="49" spans="1:9" s="12" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="29"/>
       <c r="B49" s="29"/>
       <c r="C49" s="29"/>
@@ -3718,8 +3721,9 @@
       <c r="G49" s="29"/>
       <c r="H49" s="30"/>
       <c r="I49" s="29"/>
-    </row>
-    <row r="50" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K49" s="7"/>
+    </row>
+    <row r="50" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="31" t="s">
         <v>99</v>
       </c>
@@ -3742,10 +3746,10 @@
       <c r="H50" s="32"/>
       <c r="I50" s="16"/>
     </row>
-    <row r="51" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="53" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="33" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3766,9 +3770,9 @@
       <selection sqref="A1:AI85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>-2.5780999999999998E-2</v>
       </c>
@@ -3875,7 +3879,7 @@
         <v>2.1193E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-1.7167999999999999E-2</v>
       </c>
@@ -3982,7 +3986,7 @@
         <v>1.1336000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-8.5559999999999994E-3</v>
       </c>
@@ -4089,7 +4093,7 @@
         <v>2.3340000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5.0000000000000002E-5</v>
       </c>
@@ -4196,7 +4200,7 @@
         <v>-4.3610000000000003E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6.117E-3</v>
       </c>
@@ -4303,7 +4307,7 @@
         <v>-7.6249999999999998E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7.182E-3</v>
       </c>
@@ -4410,7 +4414,7 @@
         <v>-9.7070000000000004E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4.6540000000000002E-3</v>
       </c>
@@ -4517,7 +4521,7 @@
         <v>-1.0126E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2.8370000000000001E-3</v>
       </c>
@@ -4624,7 +4628,7 @@
         <v>-9.5200000000000007E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3.9389999999999998E-3</v>
       </c>
@@ -4731,7 +4735,7 @@
         <v>-9.9399999999999992E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5.679E-3</v>
       </c>
@@ -4838,7 +4842,7 @@
         <v>-9.6399999999999993E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7.9609999999999993E-3</v>
       </c>
@@ -4945,7 +4949,7 @@
         <v>-9.2029999999999994E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8.8800000000000007E-3</v>
       </c>
@@ -5052,7 +5056,7 @@
         <v>-8.9390000000000008E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9.4479999999999998E-3</v>
       </c>
@@ -5159,7 +5163,7 @@
         <v>-8.8070000000000006E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>9.8200000000000006E-3</v>
       </c>
@@ -5266,7 +5270,7 @@
         <v>-8.3180000000000007E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1.0178E-2</v>
       </c>
@@ -5373,7 +5377,7 @@
         <v>-8.3160000000000005E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1.1164E-2</v>
       </c>
@@ -5480,7 +5484,7 @@
         <v>-7.9609999999999993E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1.1211E-2</v>
       </c>
@@ -5587,7 +5591,7 @@
         <v>-7.6880000000000004E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1.0957E-2</v>
       </c>
@@ -5694,7 +5698,7 @@
         <v>-7.3470000000000002E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1.0567E-2</v>
       </c>
@@ -5801,7 +5805,7 @@
         <v>-7.0359999999999997E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>9.6740000000000003E-3</v>
       </c>
@@ -5908,7 +5912,7 @@
         <v>-6.6239999999999997E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>9.3410000000000003E-3</v>
       </c>
@@ -6015,7 +6019,7 @@
         <v>-6.306E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>8.4539999999999997E-3</v>
       </c>
@@ -6122,7 +6126,7 @@
         <v>-5.8950000000000001E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>8.2310000000000005E-3</v>
       </c>
@@ -6229,7 +6233,7 @@
         <v>-5.509E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>7.3109999999999998E-3</v>
       </c>
@@ -6336,7 +6340,7 @@
         <v>-5.019E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6.7530000000000003E-3</v>
       </c>
@@ -6443,7 +6447,7 @@
         <v>-4.646E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6.3889999999999997E-3</v>
       </c>
@@ -6550,7 +6554,7 @@
         <v>-4.2750000000000002E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>5.8970000000000003E-3</v>
       </c>
@@ -6657,7 +6661,7 @@
         <v>-3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5.5420000000000001E-3</v>
       </c>
@@ -6764,7 +6768,7 @@
         <v>-3.4640000000000001E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>4.9880000000000002E-3</v>
       </c>
@@ -6871,7 +6875,7 @@
         <v>-3.1089999999999998E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>4.999E-3</v>
       </c>
@@ -6978,7 +6982,7 @@
         <v>-2.807E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>4.6410000000000002E-3</v>
       </c>
@@ -7085,7 +7089,7 @@
         <v>-2.444E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4.5269999999999998E-3</v>
       </c>
@@ -7192,7 +7196,7 @@
         <v>-2.173E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4.1970000000000002E-3</v>
       </c>
@@ -7299,7 +7303,7 @@
         <v>-1.92E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3.8089999999999999E-3</v>
       </c>
@@ -7406,7 +7410,7 @@
         <v>-1.7129999999999999E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3.189E-3</v>
       </c>
@@ -7513,7 +7517,7 @@
         <v>-1.567E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2.2560000000000002E-3</v>
       </c>
@@ -7620,7 +7624,7 @@
         <v>-1.438E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1.147E-3</v>
       </c>
@@ -7727,7 +7731,7 @@
         <v>-1.341E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>-4.4700000000000002E-4</v>
       </c>
@@ -7834,7 +7838,7 @@
         <v>-1.328E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>-2.1570000000000001E-3</v>
       </c>
@@ -7941,7 +7945,7 @@
         <v>-1.4239999999999999E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>-3.0799999999999998E-3</v>
       </c>
@@ -8048,7 +8052,7 @@
         <v>-1.467E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>-3.5469999999999998E-3</v>
       </c>
@@ -8155,7 +8159,7 @@
         <v>-1.64E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>-3.1150000000000001E-3</v>
       </c>
@@ -8262,7 +8266,7 @@
         <v>-1.7359999999999999E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>-5.0340000000000003E-3</v>
       </c>
@@ -8369,7 +8373,7 @@
         <v>-7.4200000000000004E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>-4.5750000000000001E-3</v>
       </c>
@@ -8476,7 +8480,7 @@
         <v>-7.5600000000000005E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>-4.5779999999999996E-3</v>
       </c>
@@ -8583,7 +8587,7 @@
         <v>-7.2400000000000003E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>-4.176E-3</v>
       </c>
@@ -8690,7 +8694,7 @@
         <v>-7.2400000000000003E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>-4.071E-3</v>
       </c>
@@ -8797,7 +8801,7 @@
         <v>-7.6000000000000004E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>-3.8679999999999999E-3</v>
       </c>
@@ -8904,7 +8908,7 @@
         <v>-7.8799999999999996E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>-3.5279999999999999E-3</v>
       </c>
@@ -9011,7 +9015,7 @@
         <v>-7.8100000000000001E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>-3.3969999999999998E-3</v>
       </c>
@@ -9118,7 +9122,7 @@
         <v>-7.6999999999999996E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>-3.4169999999999999E-3</v>
       </c>
@@ -9225,7 +9229,7 @@
         <v>-7.94E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>-3.483E-3</v>
       </c>
@@ -9332,7 +9336,7 @@
         <v>-7.9100000000000004E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>-3.454E-3</v>
       </c>
@@ -9439,7 +9443,7 @@
         <v>-7.2199999999999999E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>-3.4759999999999999E-3</v>
       </c>
@@ -9546,7 +9550,7 @@
         <v>-7.1699999999999997E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>-3.5729999999999998E-3</v>
       </c>
@@ -9653,7 +9657,7 @@
         <v>-7.2000000000000005E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>-3.666E-3</v>
       </c>
@@ -9760,7 +9764,7 @@
         <v>-6.5499999999999998E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>-3.771E-3</v>
       </c>
@@ -9867,7 +9871,7 @@
         <v>-6.4599999999999998E-4</v>
       </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>-3.8969999999999999E-3</v>
       </c>
@@ -9974,7 +9978,7 @@
         <v>-6.0800000000000003E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>-4.0460000000000001E-3</v>
       </c>
@@ -10081,7 +10085,7 @@
         <v>-6.0599999999999998E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>-4.1229999999999999E-3</v>
       </c>
@@ -10188,7 +10192,7 @@
         <v>-5.71E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>-4.4140000000000004E-3</v>
       </c>
@@ -10295,7 +10299,7 @@
         <v>-5.0500000000000002E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>-4.5139999999999998E-3</v>
       </c>
@@ -10402,7 +10406,7 @@
         <v>-4.6500000000000003E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>-4.5279999999999999E-3</v>
       </c>
@@ -10509,7 +10513,7 @@
         <v>-4.3399999999999998E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>-4.7699999999999999E-3</v>
       </c>
@@ -10616,7 +10620,7 @@
         <v>-4.0299999999999998E-4</v>
       </c>
     </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>-4.6909999999999999E-3</v>
       </c>
@@ -10723,7 +10727,7 @@
         <v>-3.4900000000000003E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>-4.9100000000000003E-3</v>
       </c>
@@ -10830,7 +10834,7 @@
         <v>-3.3E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>-4.9040000000000004E-3</v>
       </c>
@@ -10937,7 +10941,7 @@
         <v>-3.1199999999999999E-4</v>
       </c>
     </row>
-    <row r="68" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>-4.9459999999999999E-3</v>
       </c>
@@ -11044,7 +11048,7 @@
         <v>-3.1500000000000001E-4</v>
       </c>
     </row>
-    <row r="69" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>-5.2160000000000002E-3</v>
       </c>
@@ -11151,7 +11155,7 @@
         <v>-2.9100000000000003E-4</v>
       </c>
     </row>
-    <row r="70" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>-5.1619999999999999E-3</v>
       </c>
@@ -11258,7 +11262,7 @@
         <v>-2.5099999999999998E-4</v>
       </c>
     </row>
-    <row r="71" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>-5.267E-3</v>
       </c>
@@ -11365,7 +11369,7 @@
         <v>-2.6899999999999998E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>-5.3049999999999998E-3</v>
       </c>
@@ -11472,7 +11476,7 @@
         <v>-2.6699999999999998E-4</v>
       </c>
     </row>
-    <row r="73" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>-5.1419999999999999E-3</v>
       </c>
@@ -11579,7 +11583,7 @@
         <v>-2.6699999999999998E-4</v>
       </c>
     </row>
-    <row r="74" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>-5.0359999999999997E-3</v>
       </c>
@@ -11686,7 +11690,7 @@
         <v>-1.83E-4</v>
       </c>
     </row>
-    <row r="75" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>-5.3579999999999999E-3</v>
       </c>
@@ -11793,7 +11797,7 @@
         <v>-7.7999999999999999E-5</v>
       </c>
     </row>
-    <row r="76" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>-5.3299999999999997E-3</v>
       </c>
@@ -11900,7 +11904,7 @@
         <v>3.9999999999999998E-6</v>
       </c>
     </row>
-    <row r="77" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>-5.3070000000000001E-3</v>
       </c>
@@ -12007,7 +12011,7 @@
         <v>7.6000000000000004E-5</v>
       </c>
     </row>
-    <row r="78" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>-5.2009999999999999E-3</v>
       </c>
@@ -12114,7 +12118,7 @@
         <v>1.05E-4</v>
       </c>
     </row>
-    <row r="79" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>-4.8599999999999997E-3</v>
       </c>
@@ -12221,7 +12225,7 @@
         <v>1.8900000000000001E-4</v>
       </c>
     </row>
-    <row r="80" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>-4.6449999999999998E-3</v>
       </c>
@@ -12328,7 +12332,7 @@
         <v>1.3899999999999999E-4</v>
       </c>
     </row>
-    <row r="81" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>-4.365E-3</v>
       </c>
@@ -12435,7 +12439,7 @@
         <v>2.02E-4</v>
       </c>
     </row>
-    <row r="82" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>-4.7549999999999997E-3</v>
       </c>
@@ -12542,7 +12546,7 @@
         <v>2.1100000000000001E-4</v>
       </c>
     </row>
-    <row r="83" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>-4.6899999999999997E-3</v>
       </c>
@@ -12649,7 +12653,7 @@
         <v>3.3199999999999999E-4</v>
       </c>
     </row>
-    <row r="84" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>-5.0220000000000004E-3</v>
       </c>
@@ -12756,7 +12760,7 @@
         <v>3.7100000000000002E-4</v>
       </c>
     </row>
-    <row r="85" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>-5.5160000000000001E-3</v>
       </c>
@@ -12881,9 +12885,9 @@
       <selection sqref="A1:AI85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>-4.1287999999999998E-2</v>
       </c>
@@ -12990,7 +12994,7 @@
         <v>-1.4790000000000001E-3</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-4.1367000000000001E-2</v>
       </c>
@@ -13097,7 +13101,7 @@
         <v>-2.611E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-3.7718000000000002E-2</v>
       </c>
@@ -13204,7 +13208,7 @@
         <v>-1.418E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-3.5545E-2</v>
       </c>
@@ -13311,7 +13315,7 @@
         <v>-2.5010000000000002E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-3.0488999999999999E-2</v>
       </c>
@@ -13418,7 +13422,7 @@
         <v>-2.6819999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-2.7740999999999998E-2</v>
       </c>
@@ -13525,7 +13529,7 @@
         <v>-3.4970000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-2.4542999999999999E-2</v>
       </c>
@@ -13632,7 +13636,7 @@
         <v>-2.663E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-2.3806999999999998E-2</v>
       </c>
@@ -13739,7 +13743,7 @@
         <v>-3.852E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-2.1422E-2</v>
       </c>
@@ -13846,7 +13850,7 @@
         <v>-4.0220000000000004E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-2.0753000000000001E-2</v>
       </c>
@@ -13953,7 +13957,7 @@
         <v>-4.2459999999999998E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-1.8873999999999998E-2</v>
       </c>
@@ -14060,7 +14064,7 @@
         <v>-3.9769999999999996E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-1.8828999999999999E-2</v>
       </c>
@@ -14167,7 +14171,7 @@
         <v>-4.2550000000000001E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-1.8471000000000001E-2</v>
       </c>
@@ -14274,7 +14278,7 @@
         <v>-4.2909999999999997E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-1.7864000000000001E-2</v>
       </c>
@@ -14381,7 +14385,7 @@
         <v>-4.2659999999999998E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-1.7205000000000002E-2</v>
       </c>
@@ -14488,7 +14492,7 @@
         <v>-4.1949999999999999E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>-1.7103E-2</v>
       </c>
@@ -14595,7 +14599,7 @@
         <v>-4.1640000000000002E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-1.6115999999999998E-2</v>
       </c>
@@ -14702,7 +14706,7 @@
         <v>-4.267E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>-1.5507E-2</v>
       </c>
@@ -14809,7 +14813,7 @@
         <v>-4.1989999999999996E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>-1.473E-2</v>
       </c>
@@ -14916,7 +14920,7 @@
         <v>-4.15E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-1.3806000000000001E-2</v>
       </c>
@@ -15023,7 +15027,7 @@
         <v>-4.0239999999999998E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>-1.2939000000000001E-2</v>
       </c>
@@ -15130,7 +15134,7 @@
         <v>-4.0619999999999996E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>-1.2475E-2</v>
       </c>
@@ -15237,7 +15241,7 @@
         <v>-3.9150000000000001E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>-1.1646999999999999E-2</v>
       </c>
@@ -15344,7 +15348,7 @@
         <v>-3.954E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>-1.0881E-2</v>
       </c>
@@ -15451,7 +15455,7 @@
         <v>-4.0109999999999998E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>-1.0399E-2</v>
       </c>
@@ -15558,7 +15562,7 @@
         <v>-3.8639999999999998E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>-9.9030000000000003E-3</v>
       </c>
@@ -15665,7 +15669,7 @@
         <v>-3.8570000000000002E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>-9.4710000000000003E-3</v>
       </c>
@@ -15772,7 +15776,7 @@
         <v>-3.7780000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>-8.8470000000000007E-3</v>
       </c>
@@ -15879,7 +15883,7 @@
         <v>-3.908E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>-8.4019999999999997E-3</v>
       </c>
@@ -15986,7 +15990,7 @@
         <v>-3.8609999999999998E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>-7.5960000000000003E-3</v>
       </c>
@@ -16093,7 +16097,7 @@
         <v>-3.7320000000000001E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>-7.1190000000000003E-3</v>
       </c>
@@ -16200,7 +16204,7 @@
         <v>-3.8119999999999999E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>-6.5079999999999999E-3</v>
       </c>
@@ -16307,7 +16311,7 @@
         <v>-3.8159999999999999E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>-5.9249999999999997E-3</v>
       </c>
@@ -16414,7 +16418,7 @@
         <v>-3.7580000000000001E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>-5.1320000000000003E-3</v>
       </c>
@@ -16521,7 +16525,7 @@
         <v>-3.6679999999999998E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>-4.8580000000000003E-3</v>
       </c>
@@ -16628,7 +16632,7 @@
         <v>-3.5309999999999999E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>-4.9160000000000002E-3</v>
       </c>
@@ -16735,7 +16739,7 @@
         <v>-3.421E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>-5.2449999999999997E-3</v>
       </c>
@@ -16842,7 +16846,7 @@
         <v>-3.2940000000000001E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>-5.8999999999999999E-3</v>
       </c>
@@ -16949,7 +16953,7 @@
         <v>-3.0309999999999998E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>-6.7629999999999999E-3</v>
       </c>
@@ -17056,7 +17060,7 @@
         <v>-2.8449999999999999E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>-7.8220000000000008E-3</v>
       </c>
@@ -17163,7 +17167,7 @@
         <v>-2.6319999999999998E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>-8.6490000000000004E-3</v>
       </c>
@@ -17270,7 +17274,7 @@
         <v>-2.4719999999999998E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>-9.639E-3</v>
       </c>
@@ -17377,7 +17381,7 @@
         <v>-2.3349999999999998E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>-9.6080000000000002E-3</v>
       </c>
@@ -17484,7 +17488,7 @@
         <v>-1.536E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>-9.6089999999999995E-3</v>
       </c>
@@ -17591,7 +17595,7 @@
         <v>-1.469E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>-9.2999999999999992E-3</v>
       </c>
@@ -17698,7 +17702,7 @@
         <v>-1.469E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>-8.9479999999999994E-3</v>
       </c>
@@ -17805,7 +17809,7 @@
         <v>-1.4809999999999999E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>-9.0410000000000004E-3</v>
       </c>
@@ -17912,7 +17916,7 @@
         <v>-1.5330000000000001E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>-8.6440000000000006E-3</v>
       </c>
@@ -18019,7 +18023,7 @@
         <v>-1.555E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>-8.4069999999999995E-3</v>
       </c>
@@ -18126,7 +18130,7 @@
         <v>-1.66E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>-8.2459999999999999E-3</v>
       </c>
@@ -18233,7 +18237,7 @@
         <v>-1.7489999999999999E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>-8.064E-3</v>
       </c>
@@ -18340,7 +18344,7 @@
         <v>-1.7750000000000001E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>-8.2019999999999992E-3</v>
       </c>
@@ -18447,7 +18451,7 @@
         <v>-1.8450000000000001E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>-8.0560000000000007E-3</v>
       </c>
@@ -18554,7 +18558,7 @@
         <v>-1.902E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>-7.9369999999999996E-3</v>
       </c>
@@ -18661,7 +18665,7 @@
         <v>-1.933E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>-7.9690000000000004E-3</v>
       </c>
@@ -18768,7 +18772,7 @@
         <v>-1.97E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>-7.7330000000000003E-3</v>
       </c>
@@ -18875,7 +18879,7 @@
         <v>-2.0019999999999999E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>-7.7270000000000004E-3</v>
       </c>
@@ -18982,7 +18986,7 @@
         <v>-2.055E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>-7.705E-3</v>
       </c>
@@ -19089,7 +19093,7 @@
         <v>-2.088E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>-7.4609999999999998E-3</v>
       </c>
@@ -19196,7 +19200,7 @@
         <v>-2.1220000000000002E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>-7.3410000000000003E-3</v>
       </c>
@@ -19303,7 +19307,7 @@
         <v>-2.1619999999999999E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>-7.3309999999999998E-3</v>
       </c>
@@ -19410,7 +19414,7 @@
         <v>-2.1900000000000001E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>-7.1980000000000004E-3</v>
       </c>
@@ -19517,7 +19521,7 @@
         <v>-2.1710000000000002E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>-7.2509999999999996E-3</v>
       </c>
@@ -19624,7 +19628,7 @@
         <v>-2.2599999999999999E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>-7.1089999999999999E-3</v>
       </c>
@@ -19731,7 +19735,7 @@
         <v>-2.2799999999999999E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>-6.8580000000000004E-3</v>
       </c>
@@ -19838,7 +19842,7 @@
         <v>-2.3530000000000001E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>-6.986E-3</v>
       </c>
@@ -19945,7 +19949,7 @@
         <v>-2.4290000000000002E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>-6.9249999999999997E-3</v>
       </c>
@@ -20052,7 +20056,7 @@
         <v>-2.5379999999999999E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>-6.7470000000000004E-3</v>
       </c>
@@ -20159,7 +20163,7 @@
         <v>-2.5509999999999999E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>-6.8209999999999998E-3</v>
       </c>
@@ -20266,7 +20270,7 @@
         <v>-2.6580000000000002E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>-6.6490000000000004E-3</v>
       </c>
@@ -20373,7 +20377,7 @@
         <v>-2.6949999999999999E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>-6.4850000000000003E-3</v>
       </c>
@@ -20480,7 +20484,7 @@
         <v>-2.7950000000000002E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>-6.3400000000000001E-3</v>
       </c>
@@ -20587,7 +20591,7 @@
         <v>-2.9629999999999999E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>-6.1980000000000004E-3</v>
       </c>
@@ -20694,7 +20698,7 @@
         <v>-2.9659999999999999E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>-6.0150000000000004E-3</v>
       </c>
@@ -20801,7 +20805,7 @@
         <v>-2.9949999999999998E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>-5.9810000000000002E-3</v>
       </c>
@@ -20908,7 +20912,7 @@
         <v>-3.068E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>-6.1799999999999997E-3</v>
       </c>
@@ -21015,7 +21019,7 @@
         <v>-3.0019999999999999E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>-6.1149999999999998E-3</v>
       </c>
@@ -21122,7 +21126,7 @@
         <v>-2.905E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>-6.5690000000000002E-3</v>
       </c>
@@ -21229,7 +21233,7 @@
         <v>-2.8839999999999998E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>-6.6020000000000002E-3</v>
       </c>
@@ -21336,7 +21340,7 @@
         <v>-2.7650000000000001E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>-6.3099999999999996E-3</v>
       </c>
@@ -21443,7 +21447,7 @@
         <v>-2.6740000000000002E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>-6.2199999999999998E-3</v>
       </c>
@@ -21550,7 +21554,7 @@
         <v>-2.6849999999999999E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>-5.9670000000000001E-3</v>
       </c>
@@ -21657,7 +21661,7 @@
         <v>-2.689E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>-5.4429999999999999E-3</v>
       </c>
@@ -21764,7 +21768,7 @@
         <v>-2.6489999999999999E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>-4.9690000000000003E-3</v>
       </c>
@@ -21871,7 +21875,7 @@
         <v>-2.761E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>-5.0340000000000003E-3</v>
       </c>

</xml_diff>

<commit_message>
Corrected launch and recovery dates
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CE01ISSP_00004.xlsx
+++ b/deployment/Omaha_Cal_Info_CE01ISSP_00004.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="945" windowWidth="25605" windowHeight="16065" tabRatio="579" activeTab="1"/>
+    <workbookView xWindow="1875" yWindow="945" windowWidth="25605" windowHeight="16065" tabRatio="579"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -25,7 +20,7 @@
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Asset_Cal_Info!$A$1:$I$51</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -2257,8 +2252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2330,13 +2325,13 @@
         <v>4</v>
       </c>
       <c r="E2" s="40">
-        <v>42233</v>
+        <v>42230</v>
       </c>
       <c r="F2" s="41">
         <v>0.93055555555555547</v>
       </c>
       <c r="G2" s="46">
-        <v>42536</v>
+        <v>42292</v>
       </c>
       <c r="H2" s="39" t="s">
         <v>90</v>
@@ -2473,7 +2468,7 @@
   </sheetPr>
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>

</xml_diff>